<commit_message>
feat: preenchendo rodapé do relatorio
</commit_message>
<xml_diff>
--- a/Output/Relatorio_IT145632.xlsx
+++ b/Output/Relatorio_IT145632.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D367117-5F17-4D28-BA21-6A4B1A847FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E52297-4A34-4A71-AD46-CB6D490B88E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="19">
-        <v>13412.99</v>
+        <v>13417.88</v>
       </c>
       <c r="E19" s="55">
         <v>8</v>
@@ -1477,7 +1477,7 @@
       <c r="F19" s="56"/>
       <c r="G19" s="17">
         <f t="shared" si="0"/>
-        <v>107303.92</v>
+        <v>107343.03999999999</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="1"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="19">
-        <v>1823190.38</v>
+        <v>1823556.25</v>
       </c>
       <c r="E20" s="55">
         <v>1</v>
@@ -1514,7 +1514,7 @@
       <c r="F20" s="56"/>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
-        <v>1823190.38</v>
+        <v>1823556.25</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="1"/>
@@ -1754,7 +1754,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>3740457.1199999996</v>
+        <v>3740862.11</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1780,7 +1780,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>3740457.1199999996</v>
+        <v>3740862.11</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
@@ -1887,7 +1887,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>3740457.1199999996</v>
+        <v>3740862.11</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>

</xml_diff>